<commit_message>
Added in AzBio risk score
</commit_message>
<xml_diff>
--- a/Candidacy-Streamlit-Repo/performance.xlsx
+++ b/Candidacy-Streamlit-Repo/performance.xlsx
@@ -420,13 +420,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.7804144385026738</v>
+        <v>0.6858660130718954</v>
       </c>
       <c r="D2">
-        <v>0.7312325597548444</v>
+        <v>0.6211878253438364</v>
       </c>
       <c r="E2">
-        <v>0.8279488017788315</v>
+        <v>0.7468058149296148</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -437,13 +437,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.7708890374331551</v>
+        <v>0.6376633986928105</v>
       </c>
       <c r="D3">
-        <v>0.7223404699877864</v>
+        <v>0.5794586952998457</v>
       </c>
       <c r="E3">
-        <v>0.8182189235342766</v>
+        <v>0.6961786627229969</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -454,13 +454,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.755291889483066</v>
+        <v>0.6993464052287582</v>
       </c>
       <c r="D4">
-        <v>0.7047844505383594</v>
+        <v>0.6333323994747817</v>
       </c>
       <c r="E4">
-        <v>0.8056212006343308</v>
+        <v>0.7637974539586546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retrained AzBio on higher version of scikit
</commit_message>
<xml_diff>
--- a/Candidacy-Streamlit-Repo/performance.xlsx
+++ b/Candidacy-Streamlit-Repo/performance.xlsx
@@ -437,13 +437,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.6376633986928105</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="D3">
-        <v>0.5794586952998457</v>
+        <v>0.4976429989524637</v>
       </c>
       <c r="E3">
-        <v>0.6961786627229969</v>
+        <v>0.5422373153382579</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -454,13 +454,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.6993464052287582</v>
+        <v>0.7030228758169935</v>
       </c>
       <c r="D4">
-        <v>0.6333323994747817</v>
+        <v>0.6374139434025399</v>
       </c>
       <c r="E4">
-        <v>0.7637974539586546</v>
+        <v>0.7670029775506012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
necessary scikit updated related retraining
</commit_message>
<xml_diff>
--- a/Candidacy-Streamlit-Repo/performance.xlsx
+++ b/Candidacy-Streamlit-Repo/performance.xlsx
@@ -437,13 +437,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.5208333333333334</v>
+        <v>0.6376633986928105</v>
       </c>
       <c r="D3">
-        <v>0.4976429989524637</v>
+        <v>0.5794586952998457</v>
       </c>
       <c r="E3">
-        <v>0.5422373153382579</v>
+        <v>0.6961786627229969</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -454,13 +454,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.7030228758169935</v>
+        <v>0.6993464052287582</v>
       </c>
       <c r="D4">
-        <v>0.6374139434025399</v>
+        <v>0.6333323994747817</v>
       </c>
       <c r="E4">
-        <v>0.7670029775506012</v>
+        <v>0.7637974539586546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some preliminary refactoring and variable testing
</commit_message>
<xml_diff>
--- a/Candidacy-Streamlit-Repo/performance.xlsx
+++ b/Candidacy-Streamlit-Repo/performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -26,6 +26,21 @@
   </si>
   <si>
     <t>CI Upper Bound</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
   </si>
   <si>
     <t>RandomForestClassifier</t>
@@ -392,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,56 +426,116 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>0.6858660130718954</v>
+        <v>0.8263805067323644</v>
       </c>
       <c r="D2">
-        <v>0.6211878253438364</v>
+        <v>0.7883910013903975</v>
       </c>
       <c r="E2">
-        <v>0.7468058149296148</v>
+        <v>0.8630535951604434</v>
+      </c>
+      <c r="F2">
+        <v>0.9370249728555917</v>
+      </c>
+      <c r="G2">
+        <v>0.7157360406091371</v>
+      </c>
+      <c r="H2">
+        <v>0.9390642002176278</v>
+      </c>
+      <c r="I2">
+        <v>0.9370249728555917</v>
+      </c>
+      <c r="J2">
+        <v>0.9380434782608695</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>0.6376633986928105</v>
+        <v>0.8042571250626939</v>
       </c>
       <c r="D3">
-        <v>0.5794586952998457</v>
+        <v>0.7653966682008022</v>
       </c>
       <c r="E3">
-        <v>0.6961786627229969</v>
+        <v>0.8417185094358814</v>
+      </c>
+      <c r="F3">
+        <v>0.9435396308360477</v>
+      </c>
+      <c r="G3">
+        <v>0.6649746192893401</v>
+      </c>
+      <c r="H3">
+        <v>0.9294117647058824</v>
+      </c>
+      <c r="I3">
+        <v>0.9435396308360477</v>
+      </c>
+      <c r="J3">
+        <v>0.9364224137931034</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>0.6993464052287582</v>
+        <v>0.7340867628984165</v>
       </c>
       <c r="D4">
-        <v>0.6333323994747817</v>
+        <v>0.6961271644701137</v>
       </c>
       <c r="E4">
-        <v>0.7637974539586546</v>
+        <v>0.7706563481787226</v>
+      </c>
+      <c r="F4">
+        <v>0.9554831704668838</v>
+      </c>
+      <c r="G4">
+        <v>0.5126903553299492</v>
+      </c>
+      <c r="H4">
+        <v>0.9016393442622951</v>
+      </c>
+      <c r="I4">
+        <v>0.9554831704668838</v>
+      </c>
+      <c r="J4">
+        <v>0.9277807063784924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>